<commit_message>
More critical bug fixes, updateDB should be usable
* UpdateCapabilities now properly opens spreadsheet
* Changes to data spreadsheets
* Small changes to schema init script
</commit_message>
<xml_diff>
--- a/Documents/800-53-Controls-Rev4.xlsx
+++ b/Documents/800-53-Controls-Rev4.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mdl1\Documents\Cloud Security Manager\800-53-Controls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nikit\source\repos\CloudSecurityRubiksCube\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="600" yWindow="390" windowWidth="13935" windowHeight="6555"/>
+    <workbookView xWindow="600" yWindow="390" windowWidth="13935" windowHeight="6555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="800-53-controls-Rev4" sheetId="1" r:id="rId1"/>
     <sheet name="WorkingSample" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -15061,7 +15061,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -15766,6 +15766,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -15801,6 +15818,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -15976,7 +16010,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N1677"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -40181,7 +40215,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>